<commit_message>
Added plan to gitignore
</commit_message>
<xml_diff>
--- a/Vocabulary/Vocabulary.xlsx
+++ b/Vocabulary/Vocabulary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reide\OneDrive\Documents\VSCode\JavaScriptVS\LUNALA\lunala-api\server\env\Vocabulary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reide\OneDrive\Documents\VSCode\JavaScriptVS\LUNALA\lunala-api\Vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1555E26-5E03-490C-BCA9-2E4339A5E07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463D5FC5-EC48-4257-9D77-8E880EE0F804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8947" yWindow="5063" windowWidth="20678" windowHeight="14130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -4669,19 +4669,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="B325" sqref="B325"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="G177" sqref="G177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" customWidth="1"/>
-    <col min="2" max="2" width="2.73046875" customWidth="1"/>
-    <col min="3" max="3" width="2.3984375" customWidth="1"/>
-    <col min="4" max="4" width="1.73046875" customWidth="1"/>
+    <col min="1" max="1" width="9.04296875" customWidth="1"/>
+    <col min="2" max="2" width="13.58984375" customWidth="1"/>
+    <col min="3" max="3" width="27.40625" customWidth="1"/>
+    <col min="4" max="4" width="11.953125" customWidth="1"/>
+    <col min="5" max="5" width="4.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4698,7 +4699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4715,7 +4716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -4732,7 +4733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4749,7 +4750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4766,7 +4767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -4783,7 +4784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -4800,7 +4801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -4817,7 +4818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -4834,7 +4835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -4851,7 +4852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -4868,7 +4869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -4885,7 +4886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -4902,7 +4903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -4919,7 +4920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -4936,7 +4937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -4953,7 +4954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -4970,7 +4971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -4987,7 +4988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>58</v>
       </c>
@@ -5004,7 +5005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -5021,7 +5022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -5038,7 +5039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -5055,7 +5056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -5072,7 +5073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
         <v>73</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -5106,7 +5107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -5123,7 +5124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -5140,7 +5141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
         <v>85</v>
       </c>
@@ -5157,7 +5158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
         <v>88</v>
       </c>
@@ -5174,7 +5175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
         <v>91</v>
       </c>
@@ -5191,7 +5192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
         <v>94</v>
       </c>
@@ -5208,7 +5209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
         <v>97</v>
       </c>
@@ -5225,7 +5226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
         <v>100</v>
       </c>
@@ -5242,7 +5243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -5259,7 +5260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -5276,7 +5277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -5293,7 +5294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
         <v>112</v>
       </c>
@@ -5310,7 +5311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -5327,7 +5328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
         <v>118</v>
       </c>
@@ -5344,7 +5345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -5361,7 +5362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
         <v>124</v>
       </c>
@@ -5378,7 +5379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
         <v>127</v>
       </c>
@@ -5395,7 +5396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
         <v>131</v>
       </c>
@@ -5412,7 +5413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
         <v>134</v>
       </c>
@@ -5429,7 +5430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
         <v>137</v>
       </c>
@@ -5446,7 +5447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
         <v>140</v>
       </c>
@@ -5463,7 +5464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -5480,7 +5481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
         <v>146</v>
       </c>
@@ -5497,7 +5498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
         <v>149</v>
       </c>
@@ -5514,7 +5515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
         <v>152</v>
       </c>
@@ -5531,7 +5532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A51" t="s">
         <v>155</v>
       </c>
@@ -5548,7 +5549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A52" t="s">
         <v>158</v>
       </c>
@@ -5565,7 +5566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A53" t="s">
         <v>161</v>
       </c>
@@ -5582,7 +5583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A54" t="s">
         <v>164</v>
       </c>
@@ -5599,7 +5600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
         <v>167</v>
       </c>
@@ -5616,7 +5617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A56" t="s">
         <v>170</v>
       </c>
@@ -5633,7 +5634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A57" t="s">
         <v>173</v>
       </c>
@@ -5650,7 +5651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A58" t="s">
         <v>176</v>
       </c>
@@ -5667,7 +5668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -5684,7 +5685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A60" t="s">
         <v>182</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -5718,7 +5719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
         <v>188</v>
       </c>
@@ -5735,7 +5736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A63" t="s">
         <v>191</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A64" t="s">
         <v>194</v>
       </c>
@@ -5769,7 +5770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A65" t="s">
         <v>197</v>
       </c>
@@ -5786,7 +5787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A66" t="s">
         <v>200</v>
       </c>
@@ -5803,7 +5804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A67" t="s">
         <v>203</v>
       </c>
@@ -5820,7 +5821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
         <v>206</v>
       </c>
@@ -5837,7 +5838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A69" t="s">
         <v>209</v>
       </c>
@@ -5854,7 +5855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A70" t="s">
         <v>212</v>
       </c>
@@ -5871,7 +5872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A71" t="s">
         <v>215</v>
       </c>
@@ -5888,7 +5889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A72" t="s">
         <v>218</v>
       </c>
@@ -5905,7 +5906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A73" t="s">
         <v>221</v>
       </c>
@@ -5922,7 +5923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A74" t="s">
         <v>224</v>
       </c>
@@ -5939,7 +5940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A75" t="s">
         <v>227</v>
       </c>
@@ -5956,7 +5957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A76" t="s">
         <v>230</v>
       </c>
@@ -5973,7 +5974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A77" t="s">
         <v>233</v>
       </c>
@@ -5990,7 +5991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A78" t="s">
         <v>236</v>
       </c>
@@ -6007,7 +6008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A79" t="s">
         <v>239</v>
       </c>
@@ -6024,7 +6025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A80" t="s">
         <v>242</v>
       </c>
@@ -6041,7 +6042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A81" t="s">
         <v>245</v>
       </c>
@@ -6058,7 +6059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A82" t="s">
         <v>248</v>
       </c>
@@ -6075,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A83" t="s">
         <v>251</v>
       </c>
@@ -6092,7 +6093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A84" t="s">
         <v>255</v>
       </c>
@@ -6109,7 +6110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A85" t="s">
         <v>258</v>
       </c>
@@ -6126,7 +6127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A86" t="s">
         <v>261</v>
       </c>
@@ -6143,7 +6144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A87" t="s">
         <v>264</v>
       </c>
@@ -6160,7 +6161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A88" t="s">
         <v>267</v>
       </c>
@@ -6177,7 +6178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A89" t="s">
         <v>270</v>
       </c>
@@ -6194,7 +6195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A90" t="s">
         <v>273</v>
       </c>
@@ -6211,7 +6212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A91" t="s">
         <v>276</v>
       </c>
@@ -6228,7 +6229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A92" t="s">
         <v>279</v>
       </c>
@@ -6245,7 +6246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A93" t="s">
         <v>282</v>
       </c>
@@ -6262,7 +6263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A94" t="s">
         <v>285</v>
       </c>
@@ -6279,7 +6280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A95" t="s">
         <v>288</v>
       </c>
@@ -6296,7 +6297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A96" t="s">
         <v>291</v>
       </c>
@@ -6313,7 +6314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A97" t="s">
         <v>294</v>
       </c>
@@ -6330,7 +6331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A98" t="s">
         <v>297</v>
       </c>
@@ -6347,7 +6348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -6364,7 +6365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A100" t="s">
         <v>302</v>
       </c>
@@ -6381,7 +6382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A101" t="s">
         <v>305</v>
       </c>
@@ -6398,7 +6399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A102" t="s">
         <v>308</v>
       </c>
@@ -6415,7 +6416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A103" t="s">
         <v>311</v>
       </c>
@@ -6432,7 +6433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A104" t="s">
         <v>314</v>
       </c>
@@ -6449,7 +6450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A105" t="s">
         <v>317</v>
       </c>
@@ -6466,7 +6467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A106" t="s">
         <v>320</v>
       </c>
@@ -6483,7 +6484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A107" t="s">
         <v>323</v>
       </c>
@@ -6500,7 +6501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A108" t="s">
         <v>326</v>
       </c>
@@ -6517,7 +6518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A109" t="s">
         <v>329</v>
       </c>
@@ -6534,7 +6535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A110" t="s">
         <v>332</v>
       </c>
@@ -6551,7 +6552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A111" t="s">
         <v>335</v>
       </c>
@@ -6568,7 +6569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A112" t="s">
         <v>338</v>
       </c>
@@ -6585,7 +6586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A113" t="s">
         <v>341</v>
       </c>
@@ -6602,7 +6603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A114" t="s">
         <v>344</v>
       </c>
@@ -6619,7 +6620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A115" t="s">
         <v>1267</v>
       </c>
@@ -6636,7 +6637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A116" t="s">
         <v>349</v>
       </c>
@@ -6653,7 +6654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A117" t="s">
         <v>352</v>
       </c>
@@ -6670,7 +6671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A118" t="s">
         <v>355</v>
       </c>
@@ -6687,7 +6688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A119" t="s">
         <v>358</v>
       </c>
@@ -6704,7 +6705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A120" t="s">
         <v>361</v>
       </c>
@@ -6721,7 +6722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A121" t="s">
         <v>364</v>
       </c>
@@ -6738,7 +6739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A122" t="s">
         <v>367</v>
       </c>
@@ -6755,7 +6756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A123" t="s">
         <v>370</v>
       </c>
@@ -6772,7 +6773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A124" t="s">
         <v>373</v>
       </c>
@@ -6789,7 +6790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A125" t="s">
         <v>376</v>
       </c>
@@ -6806,7 +6807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A126" t="s">
         <v>379</v>
       </c>
@@ -6823,7 +6824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A127" t="s">
         <v>382</v>
       </c>
@@ -6840,7 +6841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A128" t="s">
         <v>385</v>
       </c>
@@ -6857,7 +6858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A129" t="s">
         <v>388</v>
       </c>
@@ -6874,7 +6875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A130" t="s">
         <v>391</v>
       </c>
@@ -6891,7 +6892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A131" t="s">
         <v>393</v>
       </c>
@@ -6908,7 +6909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A132" t="s">
         <v>396</v>
       </c>
@@ -6925,7 +6926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A133" t="s">
         <v>399</v>
       </c>
@@ -6942,7 +6943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A134" t="s">
         <v>402</v>
       </c>
@@ -6959,7 +6960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A135" t="s">
         <v>405</v>
       </c>
@@ -6976,7 +6977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A136" t="s">
         <v>408</v>
       </c>
@@ -6993,7 +6994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A137" t="s">
         <v>411</v>
       </c>
@@ -7010,7 +7011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A138" t="s">
         <v>414</v>
       </c>
@@ -7027,7 +7028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A139" t="s">
         <v>417</v>
       </c>
@@ -7044,7 +7045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A140" t="s">
         <v>420</v>
       </c>
@@ -7061,7 +7062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A141" t="s">
         <v>423</v>
       </c>
@@ -7078,7 +7079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A142" t="s">
         <v>426</v>
       </c>
@@ -7095,7 +7096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A143" t="s">
         <v>429</v>
       </c>
@@ -7112,7 +7113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A144" t="s">
         <v>432</v>
       </c>
@@ -7129,7 +7130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A145" t="s">
         <v>435</v>
       </c>
@@ -7146,7 +7147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A146" t="s">
         <v>438</v>
       </c>
@@ -7163,7 +7164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A147" t="s">
         <v>441</v>
       </c>
@@ -7180,7 +7181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A148" t="s">
         <v>444</v>
       </c>
@@ -7197,7 +7198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A149" t="s">
         <v>447</v>
       </c>
@@ -7214,7 +7215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A150" t="s">
         <v>450</v>
       </c>
@@ -7231,7 +7232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A151" t="s">
         <v>453</v>
       </c>
@@ -7248,7 +7249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A152" t="s">
         <v>456</v>
       </c>
@@ -7265,7 +7266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A153" t="s">
         <v>459</v>
       </c>
@@ -7282,7 +7283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A154" t="s">
         <v>462</v>
       </c>
@@ -7299,7 +7300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A155" t="s">
         <v>465</v>
       </c>
@@ -7316,7 +7317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A156" t="s">
         <v>468</v>
       </c>
@@ -7333,7 +7334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A157" t="s">
         <v>471</v>
       </c>
@@ -7350,7 +7351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A158" t="s">
         <v>474</v>
       </c>
@@ -7367,7 +7368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A159" t="s">
         <v>478</v>
       </c>
@@ -7384,7 +7385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A160" t="s">
         <v>481</v>
       </c>
@@ -7401,7 +7402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A161" t="s">
         <v>484</v>
       </c>
@@ -7418,7 +7419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A162" t="s">
         <v>487</v>
       </c>
@@ -7435,7 +7436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A163" t="s">
         <v>490</v>
       </c>
@@ -7452,7 +7453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A164" t="s">
         <v>493</v>
       </c>
@@ -7469,7 +7470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A165" t="s">
         <v>496</v>
       </c>
@@ -7486,7 +7487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A166" t="s">
         <v>499</v>
       </c>
@@ -7503,7 +7504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A167" t="s">
         <v>502</v>
       </c>
@@ -7520,7 +7521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A168" t="s">
         <v>505</v>
       </c>
@@ -7537,7 +7538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A169" t="s">
         <v>508</v>
       </c>
@@ -7554,7 +7555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A170" t="s">
         <v>511</v>
       </c>
@@ -7571,7 +7572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A171" t="s">
         <v>514</v>
       </c>
@@ -7588,7 +7589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A172" t="s">
         <v>517</v>
       </c>
@@ -7605,7 +7606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A173" t="s">
         <v>520</v>
       </c>
@@ -7622,7 +7623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A174" t="s">
         <v>523</v>
       </c>
@@ -7639,7 +7640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A175" t="s">
         <v>526</v>
       </c>
@@ -7656,7 +7657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A176" t="s">
         <v>529</v>
       </c>
@@ -7673,7 +7674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A177" t="s">
         <v>532</v>
       </c>
@@ -7690,7 +7691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A178" t="s">
         <v>535</v>
       </c>
@@ -7707,7 +7708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A179" t="s">
         <v>538</v>
       </c>
@@ -7724,7 +7725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A180" t="s">
         <v>541</v>
       </c>
@@ -7741,7 +7742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A181" t="s">
         <v>544</v>
       </c>
@@ -7758,7 +7759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A182" t="s">
         <v>546</v>
       </c>
@@ -7775,7 +7776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A183" t="s">
         <v>549</v>
       </c>
@@ -7792,7 +7793,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A184" t="s">
         <v>552</v>
       </c>
@@ -7809,7 +7810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A185" t="s">
         <v>555</v>
       </c>
@@ -7826,7 +7827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A186" t="s">
         <v>558</v>
       </c>
@@ -7843,7 +7844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A187" t="s">
         <v>561</v>
       </c>
@@ -7860,7 +7861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A188" t="s">
         <v>564</v>
       </c>
@@ -7877,7 +7878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A189" t="s">
         <v>567</v>
       </c>
@@ -7894,7 +7895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A190" t="s">
         <v>570</v>
       </c>
@@ -7911,7 +7912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A191" t="s">
         <v>573</v>
       </c>
@@ -7928,7 +7929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A192" t="s">
         <v>576</v>
       </c>
@@ -7945,7 +7946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A193" t="s">
         <v>579</v>
       </c>
@@ -7962,7 +7963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A194" t="s">
         <v>582</v>
       </c>
@@ -7979,7 +7980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A195" t="s">
         <v>585</v>
       </c>
@@ -7996,7 +7997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A196" t="s">
         <v>588</v>
       </c>
@@ -8013,7 +8014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A197" t="s">
         <v>592</v>
       </c>
@@ -8030,7 +8031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A198" t="s">
         <v>595</v>
       </c>
@@ -8047,7 +8048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A199" t="s">
         <v>595</v>
       </c>
@@ -8064,7 +8065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A200" t="s">
         <v>600</v>
       </c>
@@ -8081,7 +8082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A201" t="s">
         <v>603</v>
       </c>
@@ -8098,7 +8099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A202" t="s">
         <v>606</v>
       </c>
@@ -8115,7 +8116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A203" t="s">
         <v>609</v>
       </c>
@@ -8132,7 +8133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A204" t="s">
         <v>612</v>
       </c>
@@ -8149,7 +8150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A205" t="s">
         <v>615</v>
       </c>
@@ -8166,7 +8167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A206" t="s">
         <v>618</v>
       </c>
@@ -8183,7 +8184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A207" t="s">
         <v>621</v>
       </c>
@@ -8200,7 +8201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A208" t="s">
         <v>624</v>
       </c>
@@ -8217,7 +8218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A209" t="s">
         <v>627</v>
       </c>
@@ -8234,7 +8235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A210" t="s">
         <v>630</v>
       </c>
@@ -8251,7 +8252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A211" t="s">
         <v>633</v>
       </c>
@@ -8268,7 +8269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A212" t="s">
         <v>636</v>
       </c>
@@ -8285,7 +8286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A213" t="s">
         <v>638</v>
       </c>
@@ -8302,7 +8303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A214" t="s">
         <v>641</v>
       </c>
@@ -8319,7 +8320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A215" t="s">
         <v>644</v>
       </c>
@@ -8336,7 +8337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A216" t="s">
         <v>648</v>
       </c>
@@ -8353,7 +8354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A217" t="s">
         <v>651</v>
       </c>
@@ -8370,7 +8371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A218" t="s">
         <v>654</v>
       </c>
@@ -8387,7 +8388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A219" t="s">
         <v>657</v>
       </c>
@@ -8404,7 +8405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A220" t="s">
         <v>660</v>
       </c>
@@ -8421,7 +8422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A221" t="s">
         <v>663</v>
       </c>
@@ -8438,7 +8439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A222" t="s">
         <v>666</v>
       </c>
@@ -8455,7 +8456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A223" t="s">
         <v>669</v>
       </c>
@@ -8472,7 +8473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A224" t="s">
         <v>672</v>
       </c>
@@ -8489,7 +8490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A225" t="s">
         <v>675</v>
       </c>
@@ -8506,7 +8507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A226" t="s">
         <v>678</v>
       </c>
@@ -8523,7 +8524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A227" t="s">
         <v>681</v>
       </c>
@@ -8540,7 +8541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A228" t="s">
         <v>684</v>
       </c>
@@ -8557,7 +8558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A229" t="s">
         <v>687</v>
       </c>
@@ -8574,7 +8575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A230" t="s">
         <v>689</v>
       </c>
@@ -8591,7 +8592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A231" t="s">
         <v>692</v>
       </c>
@@ -8608,7 +8609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A232" t="s">
         <v>695</v>
       </c>
@@ -8625,7 +8626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A233" t="s">
         <v>698</v>
       </c>
@@ -8642,7 +8643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A234" t="s">
         <v>701</v>
       </c>
@@ -8659,7 +8660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A235" t="s">
         <v>704</v>
       </c>
@@ -8676,7 +8677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A236" t="s">
         <v>707</v>
       </c>
@@ -8693,7 +8694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A237" t="s">
         <v>710</v>
       </c>
@@ -8710,7 +8711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A238" t="s">
         <v>713</v>
       </c>
@@ -8727,7 +8728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A239" t="s">
         <v>716</v>
       </c>
@@ -8744,7 +8745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A240" t="s">
         <v>718</v>
       </c>
@@ -8761,7 +8762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A241" t="s">
         <v>721</v>
       </c>
@@ -8778,7 +8779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A242" t="s">
         <v>724</v>
       </c>
@@ -8795,7 +8796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A243" t="s">
         <v>727</v>
       </c>
@@ -8812,7 +8813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A244" t="s">
         <v>730</v>
       </c>
@@ -8829,7 +8830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A245" t="s">
         <v>733</v>
       </c>
@@ -8846,7 +8847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A246" t="s">
         <v>736</v>
       </c>
@@ -8863,7 +8864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A247" t="s">
         <v>739</v>
       </c>
@@ -8880,7 +8881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A248" t="s">
         <v>742</v>
       </c>
@@ -8897,7 +8898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A249" t="s">
         <v>745</v>
       </c>
@@ -8914,7 +8915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A250" t="s">
         <v>748</v>
       </c>
@@ -8931,7 +8932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A251" t="s">
         <v>750</v>
       </c>
@@ -8948,7 +8949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A252" t="s">
         <v>753</v>
       </c>
@@ -8965,7 +8966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A253" t="s">
         <v>756</v>
       </c>
@@ -8982,7 +8983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A254" t="s">
         <v>759</v>
       </c>
@@ -8999,7 +9000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A255" t="s">
         <v>762</v>
       </c>
@@ -9016,7 +9017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A256" t="s">
         <v>765</v>
       </c>
@@ -9033,7 +9034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A257" t="s">
         <v>768</v>
       </c>
@@ -9050,7 +9051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A258" t="s">
         <v>771</v>
       </c>
@@ -9067,7 +9068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A259" t="s">
         <v>774</v>
       </c>
@@ -9084,7 +9085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A260" t="s">
         <v>777</v>
       </c>
@@ -9101,7 +9102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A261" t="s">
         <v>780</v>
       </c>
@@ -9118,7 +9119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A262" t="s">
         <v>783</v>
       </c>
@@ -9135,7 +9136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A263" t="s">
         <v>786</v>
       </c>
@@ -9152,7 +9153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A264" t="s">
         <v>789</v>
       </c>
@@ -9169,7 +9170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A265" t="s">
         <v>792</v>
       </c>
@@ -9186,7 +9187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A266" t="s">
         <v>795</v>
       </c>
@@ -9203,7 +9204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A267" t="s">
         <v>798</v>
       </c>
@@ -9220,7 +9221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A268" t="s">
         <v>801</v>
       </c>
@@ -9237,7 +9238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A269" t="s">
         <v>804</v>
       </c>
@@ -9254,7 +9255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A270" t="s">
         <v>807</v>
       </c>
@@ -9271,7 +9272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A271" t="s">
         <v>810</v>
       </c>
@@ -9288,7 +9289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A272" t="s">
         <v>813</v>
       </c>
@@ -9305,7 +9306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A273" t="s">
         <v>816</v>
       </c>
@@ -9322,7 +9323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A274" t="s">
         <v>819</v>
       </c>
@@ -9339,7 +9340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A275" t="s">
         <v>822</v>
       </c>
@@ -9356,7 +9357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A276" t="s">
         <v>825</v>
       </c>
@@ -9373,7 +9374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A277" t="s">
         <v>828</v>
       </c>
@@ -9390,7 +9391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A278" t="s">
         <v>831</v>
       </c>
@@ -9407,7 +9408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A279" t="s">
         <v>834</v>
       </c>
@@ -9424,7 +9425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A280" t="s">
         <v>837</v>
       </c>
@@ -9441,7 +9442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A281" t="s">
         <v>840</v>
       </c>
@@ -9458,7 +9459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A282" t="s">
         <v>843</v>
       </c>
@@ -9475,7 +9476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A283" t="s">
         <v>846</v>
       </c>
@@ -9492,7 +9493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A284" t="s">
         <v>848</v>
       </c>
@@ -9509,7 +9510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A285" t="s">
         <v>851</v>
       </c>
@@ -9526,7 +9527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A286" t="s">
         <v>853</v>
       </c>
@@ -9543,7 +9544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A287" t="s">
         <v>856</v>
       </c>
@@ -9560,7 +9561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A288" t="s">
         <v>859</v>
       </c>
@@ -9577,7 +9578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A289" t="s">
         <v>862</v>
       </c>
@@ -9594,7 +9595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A290" t="s">
         <v>865</v>
       </c>
@@ -9611,7 +9612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A291" t="s">
         <v>868</v>
       </c>
@@ -9628,7 +9629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A292" t="s">
         <v>871</v>
       </c>
@@ -9645,7 +9646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A293" t="s">
         <v>874</v>
       </c>
@@ -9662,7 +9663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A294" t="s">
         <v>877</v>
       </c>
@@ -9679,7 +9680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A295" t="s">
         <v>880</v>
       </c>
@@ -9696,7 +9697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A296" t="s">
         <v>882</v>
       </c>
@@ -9713,7 +9714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A297" t="s">
         <v>885</v>
       </c>
@@ -9730,7 +9731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A298" t="s">
         <v>888</v>
       </c>
@@ -9747,7 +9748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A299" t="s">
         <v>891</v>
       </c>
@@ -9764,7 +9765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A300" t="s">
         <v>893</v>
       </c>
@@ -9781,7 +9782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A301" t="s">
         <v>896</v>
       </c>
@@ -9798,7 +9799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A302" t="s">
         <v>898</v>
       </c>
@@ -9815,7 +9816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A303" t="s">
         <v>901</v>
       </c>
@@ -9832,7 +9833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A304" t="s">
         <v>904</v>
       </c>
@@ -9849,7 +9850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A305" t="s">
         <v>907</v>
       </c>
@@ -9866,7 +9867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A306" t="s">
         <v>910</v>
       </c>
@@ -9883,7 +9884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A307" t="s">
         <v>913</v>
       </c>
@@ -9900,7 +9901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A308" t="s">
         <v>916</v>
       </c>
@@ -9917,7 +9918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A309" t="s">
         <v>919</v>
       </c>
@@ -9934,7 +9935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A310" t="s">
         <v>922</v>
       </c>
@@ -9951,7 +9952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A311" t="s">
         <v>925</v>
       </c>
@@ -9968,7 +9969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A312" t="s">
         <v>928</v>
       </c>
@@ -9985,7 +9986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A313" t="s">
         <v>931</v>
       </c>
@@ -10002,7 +10003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A314" t="s">
         <v>934</v>
       </c>
@@ -10019,7 +10020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A315" t="s">
         <v>937</v>
       </c>
@@ -10036,7 +10037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A316" t="s">
         <v>940</v>
       </c>
@@ -10053,7 +10054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A317" t="s">
         <v>943</v>
       </c>
@@ -10070,7 +10071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A318" t="s">
         <v>946</v>
       </c>
@@ -10087,7 +10088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A319" t="s">
         <v>949</v>
       </c>
@@ -10104,7 +10105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A320" t="s">
         <v>952</v>
       </c>
@@ -10121,7 +10122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A321" t="s">
         <v>955</v>
       </c>
@@ -10138,7 +10139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A322" t="s">
         <v>958</v>
       </c>
@@ -10155,7 +10156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A323" t="s">
         <v>961</v>
       </c>
@@ -10172,7 +10173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A324" t="s">
         <v>964</v>
       </c>
@@ -10189,7 +10190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A325" t="s">
         <v>966</v>
       </c>
@@ -10206,7 +10207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A326" t="s">
         <v>969</v>
       </c>
@@ -10223,7 +10224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A327" t="s">
         <v>972</v>
       </c>
@@ -10240,7 +10241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A328" t="s">
         <v>975</v>
       </c>
@@ -10257,7 +10258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A329" t="s">
         <v>978</v>
       </c>
@@ -10274,7 +10275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A330" t="s">
         <v>981</v>
       </c>
@@ -10291,7 +10292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A331" t="s">
         <v>984</v>
       </c>
@@ -10308,7 +10309,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A332" t="s">
         <v>987</v>
       </c>
@@ -10325,7 +10326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A333" t="s">
         <v>990</v>
       </c>
@@ -10342,7 +10343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A334" t="s">
         <v>993</v>
       </c>
@@ -10359,7 +10360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A335" t="s">
         <v>996</v>
       </c>
@@ -10376,7 +10377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A336" t="s">
         <v>999</v>
       </c>
@@ -10393,7 +10394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A337" t="s">
         <v>1002</v>
       </c>
@@ -10410,7 +10411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A338" t="s">
         <v>1005</v>
       </c>
@@ -10427,7 +10428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A339" t="s">
         <v>1008</v>
       </c>
@@ -10444,7 +10445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A340" t="s">
         <v>1011</v>
       </c>
@@ -10461,7 +10462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A341" t="s">
         <v>1014</v>
       </c>
@@ -10478,7 +10479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A342" t="s">
         <v>1017</v>
       </c>
@@ -10495,7 +10496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A343" t="s">
         <v>1020</v>
       </c>
@@ -10512,7 +10513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A344" t="s">
         <v>1023</v>
       </c>
@@ -10529,7 +10530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A345" t="s">
         <v>1026</v>
       </c>
@@ -10546,7 +10547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A346" t="s">
         <v>1029</v>
       </c>
@@ -10563,7 +10564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A347" t="s">
         <v>1032</v>
       </c>
@@ -10580,7 +10581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A348" t="s">
         <v>1035</v>
       </c>
@@ -10597,7 +10598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A349" t="s">
         <v>1038</v>
       </c>
@@ -10614,7 +10615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A350" t="s">
         <v>1041</v>
       </c>
@@ -10631,7 +10632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A351" t="s">
         <v>1044</v>
       </c>
@@ -10648,7 +10649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A352" t="s">
         <v>1047</v>
       </c>
@@ -10665,7 +10666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A353" t="s">
         <v>1050</v>
       </c>
@@ -10682,7 +10683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A354" t="s">
         <v>1053</v>
       </c>
@@ -10699,7 +10700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A355" t="s">
         <v>1056</v>
       </c>
@@ -10716,7 +10717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A356" t="s">
         <v>1059</v>
       </c>
@@ -10733,7 +10734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A357" t="s">
         <v>1062</v>
       </c>
@@ -10750,7 +10751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A358" t="s">
         <v>1065</v>
       </c>
@@ -10767,7 +10768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A359" t="s">
         <v>1068</v>
       </c>
@@ -10784,7 +10785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A360" t="s">
         <v>1071</v>
       </c>
@@ -10801,7 +10802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A361" t="s">
         <v>1074</v>
       </c>
@@ -10818,7 +10819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A362" t="s">
         <v>1077</v>
       </c>
@@ -10835,7 +10836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A363" t="s">
         <v>1080</v>
       </c>
@@ -10852,7 +10853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A364" t="s">
         <v>1083</v>
       </c>
@@ -10869,7 +10870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A365" t="s">
         <v>1086</v>
       </c>
@@ -10886,7 +10887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A366" t="s">
         <v>1088</v>
       </c>
@@ -10903,7 +10904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A367" t="s">
         <v>1090</v>
       </c>
@@ -10920,7 +10921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A368" t="s">
         <v>1093</v>
       </c>
@@ -10937,7 +10938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A369" t="s">
         <v>1096</v>
       </c>
@@ -10954,7 +10955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A370" t="s">
         <v>1099</v>
       </c>
@@ -10971,7 +10972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A371" t="s">
         <v>1102</v>
       </c>
@@ -10988,7 +10989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A372" t="s">
         <v>1105</v>
       </c>
@@ -11005,7 +11006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A373" t="s">
         <v>1108</v>
       </c>
@@ -11022,7 +11023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A374" t="s">
         <v>1111</v>
       </c>
@@ -11039,7 +11040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A375" t="s">
         <v>1113</v>
       </c>
@@ -11056,7 +11057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A376" t="s">
         <v>1116</v>
       </c>
@@ -11073,7 +11074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A377" t="s">
         <v>1119</v>
       </c>
@@ -11090,7 +11091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A378" t="s">
         <v>1122</v>
       </c>
@@ -11107,7 +11108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A379" t="s">
         <v>1125</v>
       </c>
@@ -11124,7 +11125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A380" t="s">
         <v>1128</v>
       </c>
@@ -11141,7 +11142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A381" t="s">
         <v>1131</v>
       </c>
@@ -11158,7 +11159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A382" t="s">
         <v>1134</v>
       </c>
@@ -11175,7 +11176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A383" t="s">
         <v>1137</v>
       </c>
@@ -11192,7 +11193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A384" t="s">
         <v>1140</v>
       </c>
@@ -11209,7 +11210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A385" t="s">
         <v>1143</v>
       </c>
@@ -11226,7 +11227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A386" t="s">
         <v>1146</v>
       </c>
@@ -11243,7 +11244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A387" t="s">
         <v>1149</v>
       </c>
@@ -11260,7 +11261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A388" t="s">
         <v>1152</v>
       </c>
@@ -11277,7 +11278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A389" t="s">
         <v>1155</v>
       </c>
@@ -11294,7 +11295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A390" t="s">
         <v>1158</v>
       </c>
@@ -11311,7 +11312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A391" t="s">
         <v>1161</v>
       </c>
@@ -11328,7 +11329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A392" t="s">
         <v>1164</v>
       </c>
@@ -11345,7 +11346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A393" t="s">
         <v>1167</v>
       </c>
@@ -11362,7 +11363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A394" t="s">
         <v>1169</v>
       </c>
@@ -11379,7 +11380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A395" t="s">
         <v>1172</v>
       </c>
@@ -11396,7 +11397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A396" t="s">
         <v>1175</v>
       </c>
@@ -11413,7 +11414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A397" t="s">
         <v>1177</v>
       </c>
@@ -11430,7 +11431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A398" t="s">
         <v>1180</v>
       </c>
@@ -11447,7 +11448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A399" t="s">
         <v>1183</v>
       </c>
@@ -11464,7 +11465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A400" t="s">
         <v>1186</v>
       </c>
@@ -11481,7 +11482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A401" t="s">
         <v>1189</v>
       </c>
@@ -11498,7 +11499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A402" t="s">
         <v>1192</v>
       </c>
@@ -11515,7 +11516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A403" t="s">
         <v>1195</v>
       </c>
@@ -11532,7 +11533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A404" t="s">
         <v>1198</v>
       </c>
@@ -11549,7 +11550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A405" t="s">
         <v>1201</v>
       </c>
@@ -11566,7 +11567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A406" t="s">
         <v>1204</v>
       </c>
@@ -11583,7 +11584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A407" t="s">
         <v>1207</v>
       </c>
@@ -11600,7 +11601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A408" t="s">
         <v>1210</v>
       </c>
@@ -11617,7 +11618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A409" t="s">
         <v>1213</v>
       </c>
@@ -11634,7 +11635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A410" t="s">
         <v>1216</v>
       </c>
@@ -11651,7 +11652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A411" t="s">
         <v>1219</v>
       </c>
@@ -11668,7 +11669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A412" t="s">
         <v>1222</v>
       </c>
@@ -11685,7 +11686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A413" t="s">
         <v>1225</v>
       </c>
@@ -11702,7 +11703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A414" t="s">
         <v>1228</v>
       </c>
@@ -11719,7 +11720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A415" t="s">
         <v>1231</v>
       </c>
@@ -11736,7 +11737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A416" t="s">
         <v>1234</v>
       </c>
@@ -11753,7 +11754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A417" t="s">
         <v>1237</v>
       </c>
@@ -11770,7 +11771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A418" t="s">
         <v>1240</v>
       </c>
@@ -11787,7 +11788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A419" t="s">
         <v>1243</v>
       </c>
@@ -11804,7 +11805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A420" t="s">
         <v>1246</v>
       </c>
@@ -11821,7 +11822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A421" t="s">
         <v>1249</v>
       </c>
@@ -11838,7 +11839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A422" t="s">
         <v>1252</v>
       </c>
@@ -11855,7 +11856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A423" t="s">
         <v>1255</v>
       </c>
@@ -11872,7 +11873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A424" t="s">
         <v>1266</v>
       </c>
@@ -11889,7 +11890,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A425" t="s">
         <v>1260</v>
       </c>
@@ -11906,7 +11907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A426" t="s">
         <v>1263</v>
       </c>

</xml_diff>